<commit_message>
Reformatting charts in excel for cartpole T4, T6, T7, T12, T13 and T18
</commit_message>
<xml_diff>
--- a/results/Cartpole/T12/Rewards_DDQN.xlsx
+++ b/results/Cartpole/T12/Rewards_DDQN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAA_Projecten\Q-Learning\results\Cartpole\T12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Q-Learning\results\Cartpole\T12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76E6AD31-4225-493D-A686-896E5D15FDDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8263BC0-791F-4716-AC83-F2427AFD83FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rewards_DDQN" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,16 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="1">
+  <si>
+    <t>Rewards</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -586,7 +594,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -611,6 +619,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Rewards_DDQN!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rewards</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -640,7 +659,7 @@
           </c:trendline>
           <c:val>
             <c:numRef>
-              <c:f>Rewards_DDQN!$A$1:$A$550</c:f>
+              <c:f>Rewards_DDQN!$A$2:$A$551</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="550"/>
@@ -2343,7 +2362,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2401,7 +2420,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2428,6 +2447,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2452,7 +2502,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1400" baseline="0"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3027,13 +3077,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3358,2762 +3408,2767 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A550"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A551"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57">
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63">
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64">
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66">
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67">
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68">
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69">
         <v>40</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70">
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71">
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72">
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73">
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77">
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78">
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
         <v>62</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97">
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98">
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99">
         <v>30</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100">
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101">
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102">
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103">
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104">
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105">
         <v>25</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106">
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107">
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108">
         <v>34</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109">
         <v>54</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110">
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111">
         <v>30</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112">
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113">
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114">
         <v>67</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115">
         <v>28</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116">
         <v>71</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117">
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118">
         <v>54</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119">
         <v>73</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120">
         <v>54</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121">
         <v>67</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122">
         <v>35</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123">
         <v>45</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124">
         <v>55</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125">
         <v>82</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126">
         <v>69</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127">
         <v>74</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128">
         <v>61</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129">
         <v>81</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130">
         <v>98</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131">
         <v>63</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132">
         <v>81</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133">
         <v>100</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134">
         <v>71</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135">
         <v>89</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136">
         <v>106</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138">
         <v>352</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139">
         <v>241</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140">
         <v>271</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141">
         <v>219</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142">
         <v>225</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143">
         <v>229</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144">
         <v>185</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145">
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146">
         <v>197</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148">
         <v>158</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149">
         <v>273</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150">
         <v>128</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151">
         <v>156</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152">
         <v>135</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153">
         <v>240</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154">
         <v>131</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155">
         <v>185</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156">
         <v>279</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157">
         <v>249</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158">
         <v>184</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159">
         <v>259</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160">
         <v>263</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162">
         <v>370</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163">
         <v>282</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164">
         <v>200</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165">
         <v>206</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166">
         <v>169</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168">
         <v>127</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170">
         <v>320</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171">
         <v>265</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172">
         <v>214</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174">
         <v>170</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175">
         <v>165</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176">
         <v>194</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177">
         <v>343</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178">
         <v>309</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179">
         <v>269</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180">
         <v>119</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181">
         <v>120</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182">
         <v>209</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183">
         <v>143</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184">
         <v>160</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185">
         <v>142</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186">
         <v>207</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187">
         <v>283</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>499</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>499</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>499</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>499</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>499</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>499</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>499</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>499</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>499</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>499</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>499</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>499</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>499</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>499</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>499</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>499</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>499</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>499</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>499</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208">
         <v>225</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209">
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210">
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211">
         <v>13</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212">
         <v>27</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213">
         <v>8</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216">
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217">
         <v>7</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218">
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219">
         <v>15</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220">
         <v>22</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A221">
         <v>19</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222">
         <v>58</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223">
         <v>56</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224">
         <v>91</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225">
         <v>98</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226">
         <v>144</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227">
         <v>94</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228">
         <v>87</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229">
         <v>89</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230">
         <v>183</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231">
         <v>228</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232">
         <v>279</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233">
         <v>175</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234">
         <v>196</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235">
         <v>35</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236">
         <v>179</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237">
         <v>191</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238">
         <v>135</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239">
         <v>139</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240">
         <v>151</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241">
         <v>134</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242">
         <v>129</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243">
         <v>144</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244">
         <v>161</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245">
         <v>171</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246">
         <v>172</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247">
         <v>168</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248">
         <v>175</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249">
         <v>144</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250">
         <v>141</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251">
         <v>133</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252">
         <v>139</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253">
         <v>119</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254">
         <v>139</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255">
         <v>112</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256">
         <v>116</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257">
         <v>152</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258">
         <v>141</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259">
         <v>123</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260">
         <v>133</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261">
         <v>137</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262">
         <v>128</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263">
         <v>123</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264">
         <v>138</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265">
         <v>129</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266">
         <v>140</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>127</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>127</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270">
         <v>109</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271">
         <v>139</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272">
         <v>124</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273">
         <v>65</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274">
         <v>126</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275">
         <v>189</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276">
         <v>100</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277">
         <v>143</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278">
         <v>135</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279">
         <v>153</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280">
         <v>208</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281">
         <v>175</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282">
         <v>166</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283">
         <v>153</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284">
         <v>132</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285">
         <v>143</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286">
         <v>121</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287">
         <v>141</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288">
         <v>139</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289">
         <v>141</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290">
         <v>145</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291">
         <v>154</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292">
         <v>191</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293">
         <v>148</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294">
         <v>149</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295">
         <v>191</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296">
         <v>188</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297">
         <v>184</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298">
         <v>155</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299">
         <v>177</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300">
         <v>120</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301">
         <v>114</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302">
         <v>204</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303">
         <v>145</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304">
         <v>134</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305">
         <v>175</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306">
         <v>118</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307">
         <v>253</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308">
         <v>204</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309">
         <v>186</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310">
         <v>154</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311">
         <v>224</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312">
         <v>184</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313">
         <v>253</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314">
         <v>221</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315">
         <v>218</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316">
         <v>322</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317">
         <v>227</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A318">
         <v>210</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319">
         <v>188</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A320">
         <v>206</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321">
         <v>173</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322">
         <v>193</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323">
         <v>180</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324">
         <v>191</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325">
         <v>185</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326">
         <v>182</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A327">
         <v>168</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A328">
         <v>151</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329">
         <v>162</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A330">
         <v>148</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A331">
         <v>163</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A332">
         <v>128</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A333">
         <v>170</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334">
         <v>178</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335">
         <v>186</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336">
         <v>226</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A337">
         <v>165</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A338">
         <v>181</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A339">
         <v>149</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A340">
         <v>166</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A341">
         <v>146</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A342">
         <v>169</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A343">
         <v>134</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A344">
         <v>80</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A345">
         <v>103</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A346">
         <v>124</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A347">
         <v>213</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A348">
         <v>161</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A349">
         <v>104</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A350">
         <v>266</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A351">
         <v>414</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A352">
         <v>190</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A353">
         <v>189</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A354">
         <v>212</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A355">
         <v>178</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A356">
         <v>217</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A357">
         <v>196</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A358">
         <v>220</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A359">
         <v>240</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A360">
         <v>206</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A361">
         <v>201</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A362">
         <v>269</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A363">
         <v>377</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A364">
         <v>239</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A365">
         <v>233</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A366">
         <v>203</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A367">
         <v>222</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A368">
         <v>197</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A369">
         <v>210</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A370">
         <v>203</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A371">
         <v>210</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A372">
         <v>215</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A373">
         <v>240</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A374">
         <v>279</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A376">
         <v>445</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A377">
         <v>270</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A378">
         <v>332</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A379">
         <v>307</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A380">
         <v>405</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A381">
         <v>409</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A382">
         <v>13</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A383">
         <v>194</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A384">
         <v>23</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A385">
         <v>288</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>499</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>499</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A389">
         <v>470</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>499</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>499</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>499</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>499</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>499</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>499</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>499</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>499</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>499</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>499</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>499</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>499</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>499</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>499</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>499</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>499</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>499</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>499</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>499</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>499</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>499</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>499</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>499</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>499</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A414">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A415">
         <v>139</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A416">
         <v>9</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A417">
         <v>21</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A418">
         <v>12</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A419">
         <v>11</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>10</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A422">
         <v>100</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A423">
         <v>67</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A424">
         <v>62</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A425">
         <v>211</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A426">
         <v>241</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A427">
         <v>248</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A428">
         <v>255</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A429">
         <v>273</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A429">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A430">
         <v>345</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A431">
         <v>413</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A433">
         <v>484</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A434">
         <v>327</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A435">
         <v>323</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A436">
         <v>293</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A437">
         <v>323</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A438">
         <v>251</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A439">
         <v>466</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A439">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A440">
         <v>382</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A441">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A442">
         <v>224</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A443">
         <v>113</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A444">
         <v>38</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A445">
         <v>164</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A446">
         <v>179</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A447">
         <v>168</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A448">
         <v>199</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A449">
         <v>204</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A450">
         <v>159</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A451">
         <v>161</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A452">
         <v>130</v>
       </c>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A453">
         <v>128</v>
       </c>
     </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A454">
         <v>144</v>
       </c>
     </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A455">
         <v>162</v>
       </c>
     </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A455">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A456">
         <v>39</v>
       </c>
     </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A457">
         <v>156</v>
       </c>
     </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A458">
         <v>165</v>
       </c>
     </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458">
+    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A459">
         <v>187</v>
       </c>
     </row>
-    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A460">
         <v>193</v>
       </c>
     </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A461">
         <v>221</v>
       </c>
     </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A461">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A462">
         <v>188</v>
       </c>
     </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A463">
         <v>214</v>
       </c>
     </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A464">
         <v>198</v>
       </c>
     </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A465">
         <v>165</v>
       </c>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A466">
         <v>176</v>
       </c>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A467">
         <v>182</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467">
+    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A468">
         <v>180</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A469">
         <v>165</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A470">
         <v>202</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A471">
         <v>223</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A472">
         <v>204</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A473">
         <v>189</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A474">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A475">
         <v>185</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A476">
         <v>322</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A477">
         <v>188</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A478">
         <v>173</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A479">
         <v>171</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A480">
         <v>229</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A480">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A481">
         <v>206</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A482">
         <v>183</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A482">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A483">
         <v>224</v>
       </c>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A484">
         <v>191</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A485">
         <v>185</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A486">
         <v>20</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A487">
         <v>184</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A488">
         <v>211</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A489">
         <v>264</v>
       </c>
     </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A489">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A490">
         <v>311</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A491">
         <v>398</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A491">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A492">
         <v>150</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A492">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A493">
         <v>35</v>
       </c>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A493">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A494">
         <v>58</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A494">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A495">
         <v>499</v>
       </c>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A496">
         <v>499</v>
       </c>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A497">
         <v>499</v>
       </c>
     </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A498">
         <v>499</v>
       </c>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A499">
         <v>499</v>
       </c>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A500">
         <v>499</v>
       </c>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A501">
         <v>499</v>
       </c>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A502">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A503">
         <v>164</v>
       </c>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A503">
+    <row r="504" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A504">
         <v>196</v>
       </c>
     </row>
-    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A504">
+    <row r="505" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A505">
         <v>198</v>
       </c>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A505">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A506">
         <v>211</v>
       </c>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A506">
+    <row r="507" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A507">
         <v>231</v>
       </c>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A507">
+    <row r="508" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A508">
         <v>229</v>
       </c>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A508">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A509">
         <v>251</v>
       </c>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A509">
+    <row r="510" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A510">
         <v>239</v>
       </c>
     </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A510">
+    <row r="511" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A511">
         <v>481</v>
       </c>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A511">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A512">
         <v>499</v>
       </c>
     </row>
-    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A513">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A514">
         <v>431</v>
       </c>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A514">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A515">
         <v>499</v>
       </c>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A516">
         <v>499</v>
       </c>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A517">
         <v>499</v>
       </c>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A518">
         <v>499</v>
       </c>
     </row>
-    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A519">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A520">
         <v>464</v>
       </c>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A520">
+    <row r="521" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A521">
         <v>101</v>
       </c>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A521">
+    <row r="522" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A522">
         <v>76</v>
       </c>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A522">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A523">
         <v>499</v>
       </c>
     </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A524">
         <v>499</v>
       </c>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A525">
         <v>499</v>
       </c>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A526">
         <v>499</v>
       </c>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A527">
         <v>499</v>
       </c>
     </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A528">
         <v>499</v>
       </c>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A529">
         <v>499</v>
       </c>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A530">
         <v>499</v>
       </c>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A531">
         <v>499</v>
       </c>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A532">
         <v>499</v>
       </c>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A533">
         <v>499</v>
       </c>
     </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A534">
         <v>499</v>
       </c>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A535">
         <v>499</v>
       </c>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A536">
         <v>499</v>
       </c>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A537">
         <v>499</v>
       </c>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A538">
         <v>499</v>
       </c>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A539">
         <v>499</v>
       </c>
     </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A540">
         <v>499</v>
       </c>
     </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A541">
         <v>499</v>
       </c>
     </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A542">
         <v>499</v>
       </c>
     </row>
-    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A543">
         <v>499</v>
       </c>
     </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A544">
         <v>499</v>
       </c>
     </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A545">
         <v>499</v>
       </c>
     </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A546">
         <v>499</v>
       </c>
     </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A547">
         <v>499</v>
       </c>
     </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A548">
         <v>499</v>
       </c>
     </row>
-    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A549">
         <v>499</v>
       </c>
     </row>
-    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A550">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A551">
         <v>499</v>
       </c>
     </row>

</xml_diff>